<commit_message>
agrego "pequeño formato" para proyectos de dimesiones menores que A4
</commit_message>
<xml_diff>
--- a/assets/data/projects.xlsx
+++ b/assets/data/projects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\portfolio_carabante\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85077F66-C5A5-4740-BDAE-3BD66A0FFF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9ED805-78A4-4084-BC04-C4FEFCC20166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="11380" windowHeight="13370" xr2:uid="{22BBAD9E-4F92-4AC3-93AF-C87D1CDCAAA3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="9670" xr2:uid="{22BBAD9E-4F92-4AC3-93AF-C87D1CDCAAA3}"/>
   </bookViews>
   <sheets>
     <sheet name="workbook" sheetId="1" r:id="rId1"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -605,8 +605,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrego ribbon para obra vendida
</commit_message>
<xml_diff>
--- a/assets/data/projects.xlsx
+++ b/assets/data/projects.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elias\Desktop\Cristian\Varios\vsc\portfolio_carabante\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\portfolio_carabante\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E55F88-47BF-43B5-B4E0-5FA5239B9775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="11385" windowHeight="13365"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workbook" sheetId="1" r:id="rId1"/>
     <sheet name="workbook (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -872,7 +873,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1275,44 +1276,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:J103" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:J103"/>
-  <sortState ref="A2:J100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:J103" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:J103" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J100">
     <sortCondition ref="A1:A103"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="10" name="order" dataDxfId="21"/>
-    <tableColumn id="1" name="category" dataDxfId="20"/>
-    <tableColumn id="2" name="image" dataDxfId="19"/>
-    <tableColumn id="3" name="title" dataDxfId="18"/>
-    <tableColumn id="4" name="date" dataDxfId="17"/>
-    <tableColumn id="5" name="technique" dataDxfId="16"/>
-    <tableColumn id="6" name="dimensions" dataDxfId="15"/>
-    <tableColumn id="7" name="series" dataDxfId="14"/>
-    <tableColumn id="8" name="onSale" dataDxfId="13"/>
-    <tableColumn id="9" name="awarded" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="order" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="category" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="image" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="title" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="date" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="technique" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="dimensions" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="series" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="onSale" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="awarded" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A1:J103" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J103"/>
-  <sortState ref="A2:J100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:J103" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J103" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J100">
     <sortCondition ref="A1:A103"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="10" name="order" dataDxfId="9"/>
-    <tableColumn id="1" name="category" dataDxfId="8"/>
-    <tableColumn id="2" name="image" dataDxfId="7"/>
-    <tableColumn id="3" name="title" dataDxfId="6"/>
-    <tableColumn id="4" name="date" dataDxfId="5"/>
-    <tableColumn id="5" name="technique" dataDxfId="4"/>
-    <tableColumn id="6" name="dimensions" dataDxfId="3"/>
-    <tableColumn id="7" name="series" dataDxfId="2"/>
-    <tableColumn id="8" name="onSale" dataDxfId="1"/>
-    <tableColumn id="9" name="awarded" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="order" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="category" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="image" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="title" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="date" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="technique" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="dimensions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="series" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="onSale" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="awarded" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1614,29 +1615,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD103"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>189</v>
       </c>
@@ -1668,7 +1669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1732,7 +1733,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1796,7 +1797,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1892,7 +1893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1924,7 +1925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1956,7 +1957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1988,7 +1989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2020,7 +2021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2052,7 +2053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2084,7 +2085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2116,7 +2117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F16" s="3"/>
     </row>
   </sheetData>
@@ -2129,29 +2130,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>189</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2279,7 +2280,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2343,7 +2344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2375,7 +2376,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2439,7 +2440,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2535,7 +2536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2567,7 +2568,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2599,7 +2600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2759,7 +2760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2791,7 +2792,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2823,7 +2824,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2951,7 +2952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3047,7 +3048,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3111,7 +3112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3175,7 +3176,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3198,7 +3199,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3256,7 +3257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3288,7 +3289,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3320,7 +3321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3416,7 +3417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3448,7 +3449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3512,7 +3513,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3576,7 +3577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3608,7 +3609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3640,7 +3641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3672,7 +3673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3704,7 +3705,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3736,7 +3737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3782,7 +3783,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3805,7 +3806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3828,7 +3829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3860,7 +3861,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3924,7 +3925,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3956,7 +3957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4020,7 +4021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4084,7 +4085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4113,7 +4114,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4145,7 +4146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4177,7 +4178,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4209,7 +4210,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4241,7 +4242,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4273,7 +4274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4305,7 +4306,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4337,7 +4338,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4369,7 +4370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4401,7 +4402,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4433,7 +4434,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4465,7 +4466,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4497,7 +4498,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4529,7 +4530,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4561,7 +4562,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -4593,7 +4594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -4651,7 +4652,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4680,7 +4681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4712,7 +4713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4744,7 +4745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4776,7 +4777,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4808,7 +4809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4840,7 +4841,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4872,7 +4873,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4904,7 +4905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4936,7 +4937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4968,7 +4969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5000,7 +5001,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5032,7 +5033,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5064,7 +5065,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5082,7 +5083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5100,7 +5101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5118,7 +5119,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -5136,7 +5137,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -5154,7 +5155,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -5172,7 +5173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
Elimino fecha de nacimiento y direccion. Mejoro descripción en galería
</commit_message>
<xml_diff>
--- a/assets/data/projects.xlsx
+++ b/assets/data/projects.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elias\Desktop\Cristian\Varios\vsc\portfolio_carabante\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\portfolio_carabante\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCACDCDF-0237-4022-A5F4-1DF7BE8B0880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="22620" windowHeight="13500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workbook" sheetId="1" r:id="rId1"/>
     <sheet name="workbook (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="279">
   <si>
     <t>category</t>
   </si>
@@ -863,19 +864,22 @@
     <t>terminal(3)</t>
   </si>
   <si>
-    <t>Dibujo a lápices acuarelables sobre papel 300gr. 1° Premio 2021 Salón Internacional "Juego de Damas"</t>
-  </si>
-  <si>
-    <t>1° Premio</t>
-  </si>
-  <si>
-    <t>Tintas, anilinas y lápices sobre lienzo. 1° Premio 2022 Salón Internacional "Juego de Damas"</t>
+    <t>1° Premio 2022. Salón Internacional "Juego de Damas"</t>
+  </si>
+  <si>
+    <t>1° Premio 2021. Salón Internacional "Juego de Damas"</t>
+  </si>
+  <si>
+    <t>Dibujo a lápices acuarelables sobre papel 300gr</t>
+  </si>
+  <si>
+    <t>Tintas, anilinas y lápices sobre lienzo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1325,46 +1329,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:L103" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A1:L103"/>
-  <sortState ref="A2:L103">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:L103" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:L103" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L103">
     <sortCondition ref="A1:A103"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="10" name="order" dataDxfId="23"/>
-    <tableColumn id="1" name="category" dataDxfId="22"/>
-    <tableColumn id="2" name="image" dataDxfId="21"/>
-    <tableColumn id="3" name="title" dataDxfId="20"/>
-    <tableColumn id="4" name="date" dataDxfId="19"/>
-    <tableColumn id="5" name="technique" dataDxfId="18"/>
-    <tableColumn id="6" name="dimensions" dataDxfId="17"/>
-    <tableColumn id="7" name="series" dataDxfId="16"/>
-    <tableColumn id="8" name="onSale" dataDxfId="15"/>
-    <tableColumn id="9" name="awarded" dataDxfId="14"/>
-    <tableColumn id="12" name="width" dataDxfId="13"/>
-    <tableColumn id="13" name="height" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="order" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="category" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="image" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="title" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="date" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="technique" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="dimensions" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="series" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="onSale" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="awarded" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="width" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="height" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla13" displayName="Tabla13" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J11"/>
-  <sortState ref="A2:J8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J8">
     <sortCondition ref="A1:A11"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="10" name="order" dataDxfId="9"/>
-    <tableColumn id="1" name="category" dataDxfId="8"/>
-    <tableColumn id="2" name="image" dataDxfId="7"/>
-    <tableColumn id="3" name="title" dataDxfId="6"/>
-    <tableColumn id="4" name="date" dataDxfId="5"/>
-    <tableColumn id="5" name="technique" dataDxfId="4"/>
-    <tableColumn id="6" name="dimensions" dataDxfId="3"/>
-    <tableColumn id="7" name="series" dataDxfId="2"/>
-    <tableColumn id="8" name="onSale" dataDxfId="1"/>
-    <tableColumn id="9" name="awarded" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="order" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="category" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="image" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="title" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="date" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="technique" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="dimensions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="series" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="onSale" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="awarded" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1666,31 +1670,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="85" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="3"/>
+    <col min="13" max="16384" width="11.453125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>129</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1766,7 +1770,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1804,7 +1808,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1918,7 +1922,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1956,7 +1960,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1994,7 +1998,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2032,7 +2036,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2070,7 +2074,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2108,7 +2112,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2146,7 +2150,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2222,7 +2226,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2260,7 +2264,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2298,7 +2302,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2336,7 +2340,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2412,7 +2416,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2450,7 +2454,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2488,7 +2492,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2526,7 +2530,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2564,7 +2568,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2602,7 +2606,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2640,7 +2644,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2678,7 +2682,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2716,7 +2720,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2754,7 +2758,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2792,7 +2796,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2830,7 +2834,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2868,7 +2872,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2906,7 +2910,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2935,7 +2939,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2970,7 +2974,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3005,7 +3009,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3022,7 +3026,7 @@
         <v>2022</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>73</v>
@@ -3034,7 +3038,7 @@
         <v>13</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K36" s="4">
         <v>1331</v>
@@ -3043,7 +3047,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3081,7 +3085,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3119,7 +3123,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3157,7 +3161,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3195,7 +3199,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3233,7 +3237,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3271,7 +3275,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3309,7 +3313,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3347,7 +3351,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3385,7 +3389,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3423,7 +3427,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3461,7 +3465,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3499,7 +3503,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3537,7 +3541,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3575,7 +3579,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3604,7 +3608,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3633,7 +3637,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3662,7 +3666,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3691,7 +3695,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -3729,7 +3733,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -3767,7 +3771,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -3805,7 +3809,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -3843,7 +3847,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -3881,7 +3885,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -3919,7 +3923,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -3957,7 +3961,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -3995,7 +3999,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4030,7 +4034,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -4068,7 +4072,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -4106,7 +4110,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4144,7 +4148,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4182,7 +4186,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4220,7 +4224,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4258,7 +4262,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -4296,7 +4300,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -4334,7 +4338,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -4351,7 +4355,7 @@
         <v>2021</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>122</v>
@@ -4372,7 +4376,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -4410,7 +4414,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -4448,7 +4452,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -4486,7 +4490,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -4524,7 +4528,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -4562,7 +4566,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -4600,7 +4604,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -4635,7 +4639,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -4670,7 +4674,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -4705,7 +4709,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -4743,7 +4747,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -4781,7 +4785,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -4819,7 +4823,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -4857,7 +4861,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -4895,7 +4899,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -4933,7 +4937,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -4971,7 +4975,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -5009,7 +5013,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -5047,7 +5051,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -5085,7 +5089,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -5123,7 +5127,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -5172,29 +5176,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -5226,7 +5230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>93</v>
       </c>
@@ -5244,7 +5248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>94</v>
       </c>
@@ -5262,7 +5266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>95</v>
       </c>
@@ -5280,7 +5284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>96</v>
       </c>
@@ -5298,7 +5302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>97</v>
       </c>
@@ -5316,7 +5320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>98</v>
       </c>
@@ -5334,7 +5338,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
arreglo bugs y estilos y agrego open graph
</commit_message>
<xml_diff>
--- a/assets/data/projects.xlsx
+++ b/assets/data/projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\portfolio_carabante\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCACDCDF-0237-4022-A5F4-1DF7BE8B0880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF213361-9577-4AAA-9EBA-E82907B515FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="314">
   <si>
     <t>category</t>
   </si>
@@ -874,13 +874,118 @@
   </si>
   <si>
     <t>Tintas, anilinas y lápices sobre lienzo</t>
+  </si>
+  <si>
+    <t>escultura</t>
+  </si>
+  <si>
+    <t>Modelado con arcilla roja y engobes</t>
+  </si>
+  <si>
+    <t>Retrato de Porota</t>
+  </si>
+  <si>
+    <t>Modelado en arcilla blanca, pintada con engobes</t>
+  </si>
+  <si>
+    <t>45cm altura</t>
+  </si>
+  <si>
+    <t>Niña dibujante</t>
+  </si>
+  <si>
+    <t>Modelado con arcilla roja y horneado al fuego directo</t>
+  </si>
+  <si>
+    <t>20cm altura</t>
+  </si>
+  <si>
+    <t>La emperatriz</t>
+  </si>
+  <si>
+    <t>Modelado con arcilla blanca esmaltada</t>
+  </si>
+  <si>
+    <t>Sin nombre</t>
+  </si>
+  <si>
+    <t>Modelado con arcilla roja</t>
+  </si>
+  <si>
+    <t>Retrato de Antonia</t>
+  </si>
+  <si>
+    <t>Modelado en arcilla blanca esmaltada y engobada; empotrada sobre madera</t>
+  </si>
+  <si>
+    <t>Recreación del pájaro de El Bosco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelado con masa de papel Das, en formato pequeño y pintada con acrílicos </t>
+  </si>
+  <si>
+    <t>Escultura de músico</t>
+  </si>
+  <si>
+    <t>Modelado en arcilla roja</t>
+  </si>
+  <si>
+    <t>30cm altura</t>
+  </si>
+  <si>
+    <t>Relieve en proceso</t>
+  </si>
+  <si>
+    <t>Modelado en arcilla blanca</t>
+  </si>
+  <si>
+    <t>Modelado arcilla blanca y esmaltado</t>
+  </si>
+  <si>
+    <t>retrato_de_porota</t>
+  </si>
+  <si>
+    <t>niña_dibujante</t>
+  </si>
+  <si>
+    <t>la_emperatriz</t>
+  </si>
+  <si>
+    <t>sin_nombre</t>
+  </si>
+  <si>
+    <t>retrato_de_antonia</t>
+  </si>
+  <si>
+    <t>recreación_del_pájaro_de_el_bosco</t>
+  </si>
+  <si>
+    <t>escultura_de_músico</t>
+  </si>
+  <si>
+    <t>relieve_en_proceso</t>
+  </si>
+  <si>
+    <t>perro(1)</t>
+  </si>
+  <si>
+    <t>perro(2)</t>
+  </si>
+  <si>
+    <t>perro(3)</t>
+  </si>
+  <si>
+    <t>perro(4)</t>
+  </si>
+  <si>
+    <t>Perro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,6 +1013,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -929,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -945,6 +1056,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1329,10 +1446,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:L103" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A1:L103" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L103">
-    <sortCondition ref="A1:A103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:L158" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:L158" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L158">
+    <sortCondition ref="A1:A158"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="order" dataDxfId="23"/>
@@ -1353,11 +1470,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:J11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J8">
-    <sortCondition ref="A1:A11"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla13" displayName="Tabla13" ref="A1:J16" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J16" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="10">
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="order" dataDxfId="9"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="category" dataDxfId="8"/>
@@ -1671,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="D85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1682,13 +1796,13 @@
     <col min="1" max="1" width="7" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="85" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="30.54296875" style="4" customWidth="1"/>
     <col min="11" max="11" width="9.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="11.453125" style="3"/>
@@ -5162,6 +5276,470 @@
         <v>1800</v>
       </c>
       <c r="L93" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3">
+        <v>93</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E94" s="4">
+        <v>2019</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K94" s="4">
+        <v>788</v>
+      </c>
+      <c r="L94" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3">
+        <v>94</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="E95" s="4">
+        <v>2018</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K95" s="4">
+        <v>639</v>
+      </c>
+      <c r="L95" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="3">
+        <v>95</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E96" s="4">
+        <v>2021</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K96" s="4">
+        <v>759</v>
+      </c>
+      <c r="L96" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="3">
+        <v>96</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E97" s="4">
+        <v>2022</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J97" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K97" s="4">
+        <v>639</v>
+      </c>
+      <c r="L97" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="3">
+        <v>97</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K98" s="4">
+        <v>639</v>
+      </c>
+      <c r="L98" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="3">
+        <v>98</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E99" s="4">
+        <v>2022</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J99" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K99" s="4">
+        <v>639</v>
+      </c>
+      <c r="L99" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="3">
+        <v>99</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E100" s="4">
+        <v>2021</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J100" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K100" s="4">
+        <v>1012</v>
+      </c>
+      <c r="L100" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="3">
+        <v>100</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E101" s="4">
+        <v>2020</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J101" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K101" s="4">
+        <v>639</v>
+      </c>
+      <c r="L101" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3">
+        <v>101</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E102" s="4">
+        <v>2022</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K102" s="4">
+        <v>639</v>
+      </c>
+      <c r="L102" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3">
+        <v>102</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E103" s="4">
+        <v>2022</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J103" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K103" s="4">
+        <v>759</v>
+      </c>
+      <c r="L103" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="3">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E104" s="4">
+        <v>2022</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H104" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J104" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K104" s="4">
+        <v>759</v>
+      </c>
+      <c r="L104" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="3">
+        <v>104</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E105" s="4">
+        <v>2022</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J105" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K105" s="4">
+        <v>2400</v>
+      </c>
+      <c r="L105" s="4">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A106" s="3">
+        <v>105</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="E106" s="4">
+        <v>2022</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H106" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J106" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K106" s="4">
+        <v>759</v>
+      </c>
+      <c r="L106" s="4">
         <v>1350</v>
       </c>
     </row>
@@ -5177,10 +5755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5232,129 +5810,243 @@
     </row>
     <row r="2" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_") &amp; ".jpg"</f>
-        <v>.jpg</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_") &amp; ".jpg"</f>
-        <v>.jpg</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_") &amp; ".jpg"</f>
-        <v>.jpg</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_") &amp; ".jpg"</f>
-        <v>.jpg</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_") &amp; ".jpg"</f>
-        <v>.jpg</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C7" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_") &amp; ".jpg"</f>
-        <v>.jpg</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>14</v>
-      </c>
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C8" s="1" t="str">
-        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_") &amp; ".jpg"</f>
-        <v>.jpg</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>14</v>
-      </c>
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>113</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>114</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>115</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>116</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>117</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>118</v>
+      </c>
+      <c r="C14" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>119</v>
+      </c>
+      <c r="C15" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>120</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>SUBSTITUTE(LOWER(Tabla13[[#This Row],[title]]), " ", "_")</f>
+        <v/>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>